<commit_message>
should work for not perfect gmails
</commit_message>
<xml_diff>
--- a/Programming Clubs Signup (Responses).xlsx
+++ b/Programming Clubs Signup (Responses).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gtvault-my.sharepoint.com/personal/azhang344_gatech_edu/Documents/GitHub/VirtualVisitas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{F3CC2BCA-CE0D-4BC3-8459-4DB38C428544}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F911EB74-580F-47F1-9A58-6A1CDB95E655}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{F3CC2BCA-CE0D-4BC3-8459-4DB38C428544}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3A15807C-13C8-4C2F-B50C-F32636AECEDD}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -756,15 +756,15 @@
         </r>
       </text>
     </comment>
-    <comment ref="D31" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00003A000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-          </rPr>
-          <t>YAMMID-97453531/16cc07c186ff881d</t>
+    <comment ref="D31" authorId="0" shapeId="0" xr:uid="{338FAB50-7DBB-4B71-B79A-652B3BB6D34B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t>YAMMID-97444740/16cc07bf5aea9300</t>
         </r>
       </text>
     </comment>
@@ -11657,7 +11657,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="97">
   <si>
     <t>Column D</t>
   </si>
@@ -11944,9 +11944,6 @@
     <t>sahit.mamidipaka@gmail.com</t>
   </si>
   <si>
-    <t>cyrus.m.zhou@gmail.com</t>
-  </si>
-  <si>
     <t>1100327575@fcsgaonline.org</t>
   </si>
   <si>
@@ -12044,7 +12041,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -12063,11 +12060,76 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="56">
+  <dxfs count="64">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9800"/>
+          <bgColor rgb="FFFF9800"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE06666"/>
+          <bgColor rgb="FFE06666"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFA726"/>
+          <bgColor rgb="FFFFA726"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE06666"/>
+          <bgColor rgb="FFE06666"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE06666"/>
+          <bgColor rgb="FFE06666"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6AA84F"/>
+          <bgColor rgb="FF6AA84F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF6AA84F"/>
+          <bgColor rgb="FF6AA84F"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF93C47D"/>
+          <bgColor rgb="FF93C47D"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -12833,8 +12895,8 @@
   <dimension ref="A1:F187"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -12855,7 +12917,7 @@
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -12866,9 +12928,7 @@
         <v>43698.434549791666</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
@@ -13028,9 +13088,7 @@
         <v>43698.50490133102</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
@@ -13151,7 +13209,9 @@
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
       <c r="C31" s="5"/>
-      <c r="D31" s="3"/>
+      <c r="D31" s="16" t="s">
+        <v>47</v>
+      </c>
       <c r="E31" s="6"/>
       <c r="F31" s="1"/>
     </row>
@@ -13165,42 +13225,54 @@
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="C33" s="5"/>
-      <c r="D33" s="3"/>
+      <c r="D33" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="E33" s="6"/>
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="C34" s="5"/>
-      <c r="D34" s="3"/>
+      <c r="D34" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="E34" s="6"/>
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2"/>
       <c r="C35" s="5"/>
-      <c r="D35" s="3"/>
+      <c r="D35" s="3" t="s">
+        <v>70</v>
+      </c>
       <c r="E35" s="6"/>
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
       <c r="C36" s="5"/>
-      <c r="D36" s="3"/>
+      <c r="D36" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="E36" s="6"/>
       <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="3"/>
+      <c r="D37" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="E37" s="6"/>
       <c r="F37" s="1"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="3"/>
+      <c r="D38" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="E38" s="6"/>
       <c r="F38" s="1"/>
     </row>
@@ -13354,25 +13426,19 @@
     <row r="60" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
       <c r="C60" s="13"/>
-      <c r="D60" s="10" t="s">
-        <v>72</v>
-      </c>
+      <c r="D60" s="10"/>
       <c r="F60" s="1"/>
     </row>
     <row r="61" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="2"/>
       <c r="C61" s="14"/>
-      <c r="D61" s="1" t="s">
-        <v>95</v>
-      </c>
+      <c r="D61" s="1"/>
       <c r="F61" s="1"/>
     </row>
     <row r="62" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
       <c r="C62" s="1"/>
-      <c r="D62" s="1" t="s">
-        <v>58</v>
-      </c>
+      <c r="D62" s="1"/>
       <c r="F62" s="1"/>
     </row>
     <row r="63" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
@@ -13848,53 +13914,90 @@
       <c r="C187" s="11"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:F127 A1:C1 E1:F1">
-    <cfRule type="cellIs" dxfId="55" priority="1" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="A2:F30 A1:C1 E1:F1 A32:F127 A31:C31 E31:F31">
+    <cfRule type="cellIs" dxfId="63" priority="9" stopIfTrue="1" operator="equal">
       <formula>"EMAIL_OPENED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:F127 A1:C1 E1:F1">
-    <cfRule type="cellIs" dxfId="54" priority="2" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="A2:F30 A1:C1 E1:F1 A32:F127 A31:C31 E31:F31">
+    <cfRule type="cellIs" dxfId="62" priority="10" stopIfTrue="1" operator="equal">
       <formula>"EMAIL_CLICKED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:F127 A1:C1 E1:F1">
-    <cfRule type="cellIs" dxfId="53" priority="3" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="A2:F30 A1:C1 E1:F1 A32:F127 A31:C31 E31:F31">
+    <cfRule type="cellIs" dxfId="61" priority="11" stopIfTrue="1" operator="equal">
       <formula>"RESPONDED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:F127 A1:C1 E1:F1">
-    <cfRule type="cellIs" dxfId="52" priority="4" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="A2:F30 A1:C1 E1:F1 A32:F127 A31:C31 E31:F31">
+    <cfRule type="cellIs" dxfId="60" priority="12" stopIfTrue="1" operator="equal">
       <formula>"EMAIL_NOT_SENT"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:F127 A1:C1 E1:F1">
-    <cfRule type="cellIs" dxfId="51" priority="5" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="A2:F30 A1:C1 E1:F1 A32:F127 A31:C31 E31:F31">
+    <cfRule type="cellIs" dxfId="59" priority="13" stopIfTrue="1" operator="equal">
       <formula>"BOUNCED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:F127 A1:C1 E1:F1">
-    <cfRule type="cellIs" dxfId="50" priority="6" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="A2:F30 A1:C1 E1:F1 A32:F127 A31:C31 E31:F31">
+    <cfRule type="cellIs" dxfId="58" priority="14" stopIfTrue="1" operator="equal">
       <formula>"UNSUBSCRIBED"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:F127 A1:C1 E1:F1">
-    <cfRule type="cellIs" dxfId="49" priority="7" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="A2:F30 A1:C1 E1:F1 A32:F127 A31:C31 E31:F31">
+    <cfRule type="cellIs" dxfId="57" priority="15" stopIfTrue="1" operator="equal">
       <formula>"ERROR"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:F127 A1:C1 E1:F1">
-    <cfRule type="cellIs" dxfId="48" priority="8" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="A2:F30 A1:C1 E1:F1 A32:F127 A31:C31 E31:F31">
+    <cfRule type="cellIs" dxfId="56" priority="16" stopIfTrue="1" operator="equal">
       <formula>"NO_RECIPIENT"</formula>
     </cfRule>
   </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="D60" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-  </hyperlinks>
+  <conditionalFormatting sqref="D31">
+    <cfRule type="cellIs" dxfId="7" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"EMAIL_OPENED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
+    <cfRule type="cellIs" dxfId="6" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"EMAIL_CLICKED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
+    <cfRule type="cellIs" dxfId="5" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"RESPONDED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
+    <cfRule type="cellIs" dxfId="4" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"EMAIL_NOT_SENT"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
+    <cfRule type="cellIs" dxfId="3" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"BOUNCED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
+    <cfRule type="cellIs" dxfId="2" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"UNSUBSCRIBED"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
+    <cfRule type="cellIs" dxfId="1" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"ERROR"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
+    <cfRule type="cellIs" dxfId="0" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"NO_RECIPIENT"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup fitToHeight="0" pageOrder="overThenDown" orientation="portrait" cellComments="atEnd" r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup fitToHeight="0" pageOrder="overThenDown" orientation="portrait" cellComments="atEnd" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -14462,42 +14565,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:B68">
-    <cfRule type="cellIs" dxfId="47" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="1" stopIfTrue="1" operator="equal">
       <formula>"EMAIL_OPENED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B68">
-    <cfRule type="cellIs" dxfId="46" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="2" stopIfTrue="1" operator="equal">
       <formula>"EMAIL_CLICKED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B68">
-    <cfRule type="cellIs" dxfId="45" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="3" stopIfTrue="1" operator="equal">
       <formula>"RESPONDED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B68">
-    <cfRule type="cellIs" dxfId="44" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="4" stopIfTrue="1" operator="equal">
       <formula>"EMAIL_NOT_SENT"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B68">
-    <cfRule type="cellIs" dxfId="43" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="5" stopIfTrue="1" operator="equal">
       <formula>"BOUNCED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B68">
-    <cfRule type="cellIs" dxfId="42" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="6" stopIfTrue="1" operator="equal">
       <formula>"UNSUBSCRIBED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B68">
-    <cfRule type="cellIs" dxfId="41" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="7" stopIfTrue="1" operator="equal">
       <formula>"ERROR"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B68">
-    <cfRule type="cellIs" dxfId="40" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="8" stopIfTrue="1" operator="equal">
       <formula>"NO_RECIPIENT"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15086,42 +15189,42 @@
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="A1:A64 B1:E63">
-    <cfRule type="cellIs" dxfId="39" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="1" stopIfTrue="1" operator="equal">
       <formula>"EMAIL_OPENED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A64 B1:E63">
-    <cfRule type="cellIs" dxfId="38" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="2" stopIfTrue="1" operator="equal">
       <formula>"EMAIL_CLICKED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A64 B1:E63">
-    <cfRule type="cellIs" dxfId="37" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="3" stopIfTrue="1" operator="equal">
       <formula>"RESPONDED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A64 B1:E63">
-    <cfRule type="cellIs" dxfId="36" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="4" stopIfTrue="1" operator="equal">
       <formula>"EMAIL_NOT_SENT"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A64 B1:E63">
-    <cfRule type="cellIs" dxfId="35" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="5" stopIfTrue="1" operator="equal">
       <formula>"BOUNCED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A64 B1:E63">
-    <cfRule type="cellIs" dxfId="34" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="6" stopIfTrue="1" operator="equal">
       <formula>"UNSUBSCRIBED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A64 B1:E63">
-    <cfRule type="cellIs" dxfId="33" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="7" stopIfTrue="1" operator="equal">
       <formula>"ERROR"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A64 B1:E63">
-    <cfRule type="cellIs" dxfId="32" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="8" stopIfTrue="1" operator="equal">
       <formula>"NO_RECIPIENT"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15693,42 +15796,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1 F1:F62 A3:A62 A64">
-    <cfRule type="cellIs" dxfId="31" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="1" stopIfTrue="1" operator="equal">
       <formula>"EMAIL_OPENED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1 F1:F62 A3:A62 A64">
-    <cfRule type="cellIs" dxfId="30" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="2" stopIfTrue="1" operator="equal">
       <formula>"EMAIL_CLICKED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1 F1:F62 A3:A62 A64">
-    <cfRule type="cellIs" dxfId="29" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="3" stopIfTrue="1" operator="equal">
       <formula>"RESPONDED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1 F1:F62 A3:A62 A64">
-    <cfRule type="cellIs" dxfId="28" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="4" stopIfTrue="1" operator="equal">
       <formula>"EMAIL_NOT_SENT"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1 F1:F62 A3:A62 A64">
-    <cfRule type="cellIs" dxfId="27" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="5" stopIfTrue="1" operator="equal">
       <formula>"BOUNCED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1 F1:F62 A3:A62 A64">
-    <cfRule type="cellIs" dxfId="26" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="6" stopIfTrue="1" operator="equal">
       <formula>"UNSUBSCRIBED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1 F1:F62 A3:A62 A64">
-    <cfRule type="cellIs" dxfId="25" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="7" stopIfTrue="1" operator="equal">
       <formula>"ERROR"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1 F1:F62 A3:A62 A64">
-    <cfRule type="cellIs" dxfId="24" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="8" stopIfTrue="1" operator="equal">
       <formula>"NO_RECIPIENT"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16317,42 +16420,42 @@
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="A1:E64">
-    <cfRule type="cellIs" dxfId="23" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="1" stopIfTrue="1" operator="equal">
       <formula>"EMAIL_OPENED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:E64">
-    <cfRule type="cellIs" dxfId="22" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="2" stopIfTrue="1" operator="equal">
       <formula>"EMAIL_CLICKED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:E64">
-    <cfRule type="cellIs" dxfId="21" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="3" stopIfTrue="1" operator="equal">
       <formula>"RESPONDED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:E64">
-    <cfRule type="cellIs" dxfId="20" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="4" stopIfTrue="1" operator="equal">
       <formula>"EMAIL_NOT_SENT"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:E64">
-    <cfRule type="cellIs" dxfId="19" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="5" stopIfTrue="1" operator="equal">
       <formula>"BOUNCED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:E64">
-    <cfRule type="cellIs" dxfId="18" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="6" stopIfTrue="1" operator="equal">
       <formula>"UNSUBSCRIBED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:E64">
-    <cfRule type="cellIs" dxfId="17" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="7" stopIfTrue="1" operator="equal">
       <formula>"ERROR"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:E64">
-    <cfRule type="cellIs" dxfId="16" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="8" stopIfTrue="1" operator="equal">
       <formula>"NO_RECIPIENT"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16908,7 +17011,7 @@
     </row>
     <row r="63" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>28</v>
@@ -16916,42 +17019,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:B63">
-    <cfRule type="cellIs" dxfId="15" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="1" stopIfTrue="1" operator="equal">
       <formula>"EMAIL_OPENED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B63">
-    <cfRule type="cellIs" dxfId="14" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="2" stopIfTrue="1" operator="equal">
       <formula>"EMAIL_CLICKED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B63">
-    <cfRule type="cellIs" dxfId="13" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="3" stopIfTrue="1" operator="equal">
       <formula>"RESPONDED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B63">
-    <cfRule type="cellIs" dxfId="12" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="4" stopIfTrue="1" operator="equal">
       <formula>"EMAIL_NOT_SENT"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B63">
-    <cfRule type="cellIs" dxfId="11" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="5" stopIfTrue="1" operator="equal">
       <formula>"BOUNCED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B63">
-    <cfRule type="cellIs" dxfId="10" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="6" stopIfTrue="1" operator="equal">
       <formula>"UNSUBSCRIBED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B63">
-    <cfRule type="cellIs" dxfId="9" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="7" stopIfTrue="1" operator="equal">
       <formula>"ERROR"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B63">
-    <cfRule type="cellIs" dxfId="8" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="8" stopIfTrue="1" operator="equal">
       <formula>"NO_RECIPIENT"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17547,42 +17650,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:B67">
-    <cfRule type="cellIs" dxfId="7" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="1" stopIfTrue="1" operator="equal">
       <formula>"EMAIL_OPENED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B67">
-    <cfRule type="cellIs" dxfId="6" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" stopIfTrue="1" operator="equal">
       <formula>"EMAIL_CLICKED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B67">
-    <cfRule type="cellIs" dxfId="5" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="3" stopIfTrue="1" operator="equal">
       <formula>"RESPONDED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B67">
-    <cfRule type="cellIs" dxfId="4" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="4" stopIfTrue="1" operator="equal">
       <formula>"EMAIL_NOT_SENT"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B67">
-    <cfRule type="cellIs" dxfId="3" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" stopIfTrue="1" operator="equal">
       <formula>"BOUNCED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B67">
-    <cfRule type="cellIs" dxfId="2" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="6" stopIfTrue="1" operator="equal">
       <formula>"UNSUBSCRIBED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B67">
-    <cfRule type="cellIs" dxfId="1" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="7" stopIfTrue="1" operator="equal">
       <formula>"ERROR"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:B67">
-    <cfRule type="cellIs" dxfId="0" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="8" stopIfTrue="1" operator="equal">
       <formula>"NO_RECIPIENT"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>